<commit_message>
jcb log indrayani changu 4.3hr, panchakanya valuation, kalimasta valuation given
</commit_message>
<xml_diff>
--- a/ofc/estimates/Finalized valuations/pahiro bipad dozer/jcb log इन्द्रायणी चाँगु सडक पहिरो.xlsx
+++ b/ofc/estimates/Finalized valuations/pahiro bipad dozer/jcb log इन्द्रायणी चाँगु सडक पहिरो.xlsx
@@ -9,16 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ESTIMATE (3)" sheetId="1" r:id="rId1"/>
     <sheet name="ओन्ली सचिब" sheetId="2" r:id="rId2"/>
+    <sheet name="include sthaniya" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'ESTIMATE (3)'!$A$1:$H$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'include sthaniya'!$A$1:$H$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'ओन्ली सचिब'!$A$1:$H$22</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'ESTIMATE (3)'!$1:$11</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'include sthaniya'!$1:$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'ओन्ली सचिब'!$1:$11</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>सुरु घण्टा मिटर (क)</t>
   </si>
@@ -127,6 +130,27 @@
   </si>
   <si>
     <t>वडा प्राविधिकको नाम / सहि</t>
+  </si>
+  <si>
+    <t xml:space="preserve">मितिः                          </t>
+  </si>
+  <si>
+    <t>स्थानीयको नाम / सहि</t>
+  </si>
+  <si>
+    <t>............................</t>
+  </si>
+  <si>
+    <t>वडा अधक्ष्यको सहि</t>
+  </si>
+  <si>
+    <t>वडा सदस्यको सहि</t>
+  </si>
+  <si>
+    <t xml:space="preserve">फर्म्/व्यक्तिको नाम : न्यू माता इन्द्रायणी कन्स्ट्रक सन सर्भिस </t>
+  </si>
+  <si>
+    <t>...............................</t>
   </si>
 </sst>
 </file>
@@ -298,7 +322,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -364,6 +388,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,8 +406,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -664,7 +700,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G12" sqref="G12:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -681,50 +717,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="45">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="27">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="27">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" ht="35.25">
       <c r="A5" s="18"/>
@@ -737,23 +773,23 @@
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -773,11 +809,11 @@
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" ht="34.5">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
@@ -1002,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1020,50 +1056,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="45">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="27">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="27">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" ht="35.25">
       <c r="A5" s="18"/>
@@ -1076,23 +1112,23 @@
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -1112,11 +1148,11 @@
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" ht="34.5">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
@@ -1288,6 +1324,356 @@
       </c>
       <c r="E27" s="4" t="str">
         <f>E26</f>
+        <v>without vat</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="63" fitToHeight="2" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="7" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="27" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="45">
+      <c r="A2" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:8" ht="27">
+      <c r="A3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" ht="27">
+      <c r="A4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="35.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:8" ht="33.75" customHeight="1">
+      <c r="A6" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+    </row>
+    <row r="7" spans="1:8" ht="33.75" customHeight="1">
+      <c r="A7" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" ht="33.75" customHeight="1">
+      <c r="A8" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" ht="34.5">
+      <c r="A9" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" ht="33">
+      <c r="E10" s="22"/>
+      <c r="H10" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="40.5">
+      <c r="A11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="65.25" customHeight="1">
+      <c r="A12" s="9">
+        <v>1</v>
+      </c>
+      <c r="B12" s="15">
+        <v>66367</v>
+      </c>
+      <c r="C12" s="35">
+        <v>4300</v>
+      </c>
+      <c r="D12" s="36">
+        <v>4304.3</v>
+      </c>
+      <c r="E12" s="36">
+        <v>4.3</v>
+      </c>
+      <c r="F12" s="37">
+        <v>2198</v>
+      </c>
+      <c r="G12" s="1">
+        <f>F12*E12</f>
+        <v>9451.4</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="2">
+        <f>SUM(G12:G12)</f>
+        <v>9451.4</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="2">
+        <f>G13</f>
+        <v>9451.4</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="2">
+        <f>0.13*G15</f>
+        <v>1228.682</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="2">
+        <f>SUM(G15:G16)</f>
+        <v>10680.082</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="21" spans="1:8" ht="20.25">
+      <c r="B21" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="20.25">
+      <c r="B22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="1:8" ht="18.75">
+      <c r="B23" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="20.25">
+      <c r="C29" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="20.25">
+      <c r="C30" s="26"/>
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" ht="18.75">
+      <c r="C31" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="28"/>
+      <c r="E31" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
+      <c r="C36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5">
+      <c r="C37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="4" t="str">
+        <f>E36</f>
         <v>without vat</v>
       </c>
     </row>

</xml_diff>